<commit_message>
added new files and readjusted batch size
</commit_message>
<xml_diff>
--- a/ID-overview.xlsx
+++ b/ID-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Q&amp;U Project\SLOTest_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C4D671-8B94-4C62-9FBF-42956C58DCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5FEEB0-AAB3-49D3-BD20-9BEFB023DE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="2835" windowWidth="17610" windowHeight="15600" xr2:uid="{EC8FBFC7-18FE-46A4-9E47-55AF37D8947C}"/>
+    <workbookView xWindow="10695" yWindow="0" windowWidth="17610" windowHeight="15600" xr2:uid="{EC8FBFC7-18FE-46A4-9E47-55AF37D8947C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,7 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -883,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3A7295-C86C-49BE-8C70-E8D36DAA591A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,39 +912,39 @@
         <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>108</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>107</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>107</v>
       </c>
     </row>
@@ -960,28 +959,28 @@
         <v>109</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="4" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="4" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>106</v>
@@ -999,28 +998,28 @@
         <v>110</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="4" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>106</v>
@@ -1038,28 +1037,28 @@
         <v>111</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>106</v>
@@ -1077,28 +1076,28 @@
         <v>112</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="4" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="4" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>106</v>
@@ -1116,28 +1115,28 @@
         <v>113</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>106</v>
@@ -1155,28 +1154,28 @@
         <v>114</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="4" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="4" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>106</v>
@@ -1194,28 +1193,28 @@
         <v>115</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="4" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>106</v>
@@ -1231,28 +1230,28 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="4" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="4" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>106</v>
@@ -1268,28 +1267,28 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="4" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>106</v>
@@ -1305,28 +1304,28 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="4" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>106</v>
@@ -1342,28 +1341,28 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="4" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>106</v>
@@ -1379,28 +1378,28 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="4" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="4" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>106</v>
@@ -1416,28 +1415,28 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="4" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>106</v>
@@ -1453,28 +1452,28 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="4" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="4" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>106</v>
@@ -1490,28 +1489,28 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="4" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="4" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>106</v>
@@ -1527,28 +1526,28 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="4" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="4" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>106</v>
@@ -1564,28 +1563,28 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="4" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="4" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
@@ -1601,28 +1600,28 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="4" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="4" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>106</v>
@@ -1638,28 +1637,28 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="4" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>106</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="4" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>106</v>
@@ -1675,28 +1674,28 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="6" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>106</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="6" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>106</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>106</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="6" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>106</v>

</xml_diff>